<commit_message>
added sample feedback xl files for testing
</commit_message>
<xml_diff>
--- a/Feedback.xlsx
+++ b/Feedback.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287638\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287638\Desktop\CAPSTONE_PROJECT\CAPSTONE_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2A8C1F-7030-42BF-B44A-10FAFA71C81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868BA39A-B820-49CC-9E3E-FD2F0398A905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AEF08C7D-BD4A-4081-9006-A02F6CFA0369}"/>
   </bookViews>
@@ -36,35 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Design ID</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Rating</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>alice</t>
-  </si>
-  <si>
-    <t>bobboy</t>
-  </si>
-  <si>
-    <t>charlie</t>
-  </si>
-  <si>
-    <t>basith</t>
-  </si>
-  <si>
-    <t>chaitanya</t>
-  </si>
-  <si>
     <t>loved the design!</t>
   </si>
   <si>
@@ -74,10 +50,13 @@
     <t>Didn’t like it much</t>
   </si>
   <si>
-    <t>good , but</t>
-  </si>
-  <si>
-    <t>poor design</t>
+    <t>Feedback ID</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -429,96 +408,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECCD7C9-81C9-4FE0-9212-CAE92AB3C06A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>